<commit_message>
BCPSDEMS-530 v1.19 mapping changes
</commit_message>
<xml_diff>
--- a/mapping/docs/Tracking DEMS Integration Data Mapping v1.20.xlsx
+++ b/mapping/docs/Tracking DEMS Integration Data Mapping v1.20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/git/jade/jpss-jade-ccm/mapping/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EB52E2-A08C-8F4C-8BE8-566342527134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916E531A-5E82-764A-93A4-D530B479522F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0. Change Log" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2571" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2574" uniqueCount="856">
   <si>
     <t>Change Date</t>
   </si>
@@ -4036,7 +4036,10 @@
     <t>QUESTION: Not updated; this implies use of concatenated names instead of MAPID 23</t>
   </si>
   <si>
-    <t>STOPPED HERE..</t>
+    <t>Always associate an accused to a case with ParticipantType = "Accused"</t>
+  </si>
+  <si>
+    <t>Already done.  Previous issues with DEMS API</t>
   </si>
 </sst>
 </file>
@@ -4049,7 +4052,7 @@
     <numFmt numFmtId="166" formatCode="dd/mmm/yyyy"/>
     <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ h:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4244,14 +4247,6 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4524,7 +4519,7 @@
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4853,9 +4848,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -6300,14 +6292,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A292DBCF-B35F-4E38-91EC-93A3024A386F}" name="Table2" displayName="Table2" ref="A1:W121" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23" headerRowCellStyle="Good">
-  <autoFilter ref="A1:W121" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="V1.19"/>
-        <filter val="V1.20"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:W121" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{835DEB9C-EF50-49F3-AADC-8EEC259AD441}" name="#" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{8E79AED4-9838-4FD0-9B84-9FCF2119C980}" name="Status" dataDxfId="21"/>
@@ -7295,11 +7280,11 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:X121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F109" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="O112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K116" sqref="K116"/>
+      <selection pane="bottomRight" activeCell="O114" sqref="O114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -7399,7 +7384,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:23" customFormat="1" ht="48" hidden="1">
+    <row r="2" spans="1:23" customFormat="1" ht="48">
       <c r="A2" s="58">
         <v>1</v>
       </c>
@@ -7535,7 +7520,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="4" spans="1:23" customFormat="1" ht="80" hidden="1">
+    <row r="4" spans="1:23" customFormat="1" ht="80">
       <c r="A4" s="58">
         <v>3</v>
       </c>
@@ -7590,7 +7575,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:23" customFormat="1" ht="16" hidden="1">
+    <row r="5" spans="1:23" customFormat="1" ht="16">
       <c r="A5" s="58">
         <v>4</v>
       </c>
@@ -7641,7 +7626,7 @@
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:23" customFormat="1" ht="272" hidden="1">
+    <row r="6" spans="1:23" customFormat="1" ht="272">
       <c r="A6" s="58">
         <v>5</v>
       </c>
@@ -7710,7 +7695,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:23" customFormat="1" ht="256" hidden="1">
+    <row r="7" spans="1:23" customFormat="1" ht="256">
       <c r="A7" s="58">
         <v>6</v>
       </c>
@@ -7779,7 +7764,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:23" customFormat="1" ht="128" hidden="1">
+    <row r="8" spans="1:23" customFormat="1" ht="128">
       <c r="A8" s="58">
         <v>7</v>
       </c>
@@ -7848,7 +7833,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="112" hidden="1">
+    <row r="9" spans="1:23" ht="112">
       <c r="A9" s="58">
         <v>8</v>
       </c>
@@ -7917,7 +7902,7 @@
       </c>
       <c r="W9" s="6"/>
     </row>
-    <row r="10" spans="1:23" ht="32" hidden="1">
+    <row r="10" spans="1:23" ht="32">
       <c r="A10" s="58">
         <v>9</v>
       </c>
@@ -7984,7 +7969,7 @@
       </c>
       <c r="W10" s="6"/>
     </row>
-    <row r="11" spans="1:23" ht="32" hidden="1">
+    <row r="11" spans="1:23" ht="32">
       <c r="A11" s="58">
         <v>10</v>
       </c>
@@ -8051,7 +8036,7 @@
       </c>
       <c r="W11" s="6"/>
     </row>
-    <row r="12" spans="1:23" ht="96" hidden="1">
+    <row r="12" spans="1:23" ht="96">
       <c r="A12" s="58">
         <v>11</v>
       </c>
@@ -8118,7 +8103,7 @@
       </c>
       <c r="W12" s="6"/>
     </row>
-    <row r="13" spans="1:23" ht="128" hidden="1">
+    <row r="13" spans="1:23" ht="128">
       <c r="A13" s="84">
         <v>12</v>
       </c>
@@ -8187,7 +8172,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="14" spans="1:23" customFormat="1" ht="128" hidden="1">
+    <row r="14" spans="1:23" customFormat="1" ht="128">
       <c r="A14" s="84">
         <v>13</v>
       </c>
@@ -8256,7 +8241,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="15" spans="1:23" customFormat="1" ht="32" hidden="1">
+    <row r="15" spans="1:23" customFormat="1" ht="32">
       <c r="A15" s="58">
         <v>14</v>
       </c>
@@ -8392,7 +8377,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="1:23" customFormat="1" ht="80" hidden="1">
+    <row r="17" spans="1:23" customFormat="1" ht="80">
       <c r="A17" s="58">
         <v>16</v>
       </c>
@@ -8459,7 +8444,7 @@
       </c>
       <c r="W17" s="6"/>
     </row>
-    <row r="18" spans="1:23" customFormat="1" ht="144" hidden="1">
+    <row r="18" spans="1:23" customFormat="1" ht="144">
       <c r="A18" s="58">
         <v>17</v>
       </c>
@@ -8526,7 +8511,7 @@
       </c>
       <c r="W18" s="59"/>
     </row>
-    <row r="19" spans="1:23" customFormat="1" ht="112" hidden="1">
+    <row r="19" spans="1:23" customFormat="1" ht="112">
       <c r="A19" s="58">
         <v>18</v>
       </c>
@@ -8593,7 +8578,7 @@
       </c>
       <c r="W19" s="6"/>
     </row>
-    <row r="20" spans="1:23" customFormat="1" ht="288" hidden="1">
+    <row r="20" spans="1:23" customFormat="1" ht="288">
       <c r="A20" s="58">
         <v>19</v>
       </c>
@@ -8662,7 +8647,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:23" customFormat="1" ht="335" hidden="1">
+    <row r="21" spans="1:23" customFormat="1" ht="335">
       <c r="A21" s="58">
         <v>20</v>
       </c>
@@ -8731,7 +8716,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="22" spans="1:23" customFormat="1" ht="96" hidden="1">
+    <row r="22" spans="1:23" customFormat="1" ht="96">
       <c r="A22" s="58">
         <v>21</v>
       </c>
@@ -8796,7 +8781,7 @@
       </c>
       <c r="W22" s="9"/>
     </row>
-    <row r="23" spans="1:23" customFormat="1" ht="80" hidden="1">
+    <row r="23" spans="1:23" customFormat="1" ht="80">
       <c r="A23" s="63">
         <v>22</v>
       </c>
@@ -8930,7 +8915,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="25" spans="1:23" customFormat="1" ht="256" hidden="1">
+    <row r="25" spans="1:23" customFormat="1" ht="256">
       <c r="A25" s="93">
         <v>24</v>
       </c>
@@ -8999,7 +8984,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="26" spans="1:23" customFormat="1" ht="80" hidden="1">
+    <row r="26" spans="1:23" customFormat="1" ht="80">
       <c r="A26" s="58">
         <v>25</v>
       </c>
@@ -9065,7 +9050,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:23" customFormat="1" ht="256" hidden="1">
+    <row r="27" spans="1:23" customFormat="1" ht="256">
       <c r="A27" s="58">
         <v>26</v>
       </c>
@@ -9132,7 +9117,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="28" spans="1:23" customFormat="1" ht="96" hidden="1">
+    <row r="28" spans="1:23" customFormat="1" ht="96">
       <c r="A28" s="84">
         <v>27</v>
       </c>
@@ -9201,7 +9186,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="29" spans="1:23" customFormat="1" ht="32" hidden="1">
+    <row r="29" spans="1:23" customFormat="1" ht="32">
       <c r="A29" s="63">
         <v>28</v>
       </c>
@@ -9264,7 +9249,7 @@
       <c r="V29" s="6"/>
       <c r="W29" s="9"/>
     </row>
-    <row r="30" spans="1:23" customFormat="1" ht="48" hidden="1">
+    <row r="30" spans="1:23" customFormat="1" ht="48">
       <c r="A30" s="95">
         <v>29</v>
       </c>
@@ -9333,7 +9318,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="31" spans="1:23" customFormat="1" ht="128" hidden="1">
+    <row r="31" spans="1:23" customFormat="1" ht="128">
       <c r="A31" s="93">
         <v>30</v>
       </c>
@@ -9402,7 +9387,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:23" customFormat="1" ht="208" hidden="1">
+    <row r="32" spans="1:23" customFormat="1" ht="208">
       <c r="A32" s="58">
         <v>31</v>
       </c>
@@ -9467,7 +9452,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="33" spans="1:24" s="6" customFormat="1" ht="192" hidden="1">
+    <row r="33" spans="1:24" s="6" customFormat="1" ht="192">
       <c r="A33" s="58">
         <v>32</v>
       </c>
@@ -9537,7 +9522,7 @@
       </c>
       <c r="X33" s="90"/>
     </row>
-    <row r="34" spans="1:24" customFormat="1" ht="112" hidden="1">
+    <row r="34" spans="1:24" customFormat="1" ht="112">
       <c r="A34" s="58">
         <v>33</v>
       </c>
@@ -9606,7 +9591,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="35" spans="1:24" customFormat="1" ht="176" hidden="1">
+    <row r="35" spans="1:24" customFormat="1" ht="176">
       <c r="A35" s="58">
         <v>34</v>
       </c>
@@ -9675,7 +9660,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="36" spans="1:24" customFormat="1" ht="112" hidden="1">
+    <row r="36" spans="1:24" customFormat="1" ht="112">
       <c r="A36" s="58">
         <v>35</v>
       </c>
@@ -9742,7 +9727,7 @@
       </c>
       <c r="W36" s="6"/>
     </row>
-    <row r="37" spans="1:24" customFormat="1" ht="160" hidden="1">
+    <row r="37" spans="1:24" customFormat="1" ht="160">
       <c r="A37" s="58">
         <v>36</v>
       </c>
@@ -9809,7 +9794,7 @@
       </c>
       <c r="W37" s="6"/>
     </row>
-    <row r="38" spans="1:24" customFormat="1" ht="32" hidden="1">
+    <row r="38" spans="1:24" customFormat="1" ht="32">
       <c r="A38" s="58">
         <v>37</v>
       </c>
@@ -9876,7 +9861,7 @@
       </c>
       <c r="W38" s="6"/>
     </row>
-    <row r="39" spans="1:24" customFormat="1" ht="356" hidden="1">
+    <row r="39" spans="1:24" customFormat="1" ht="356">
       <c r="A39" s="58">
         <v>38</v>
       </c>
@@ -9945,7 +9930,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="40" spans="1:24" customFormat="1" ht="240" hidden="1">
+    <row r="40" spans="1:24" customFormat="1" ht="240">
       <c r="A40" s="58">
         <v>39</v>
       </c>
@@ -10012,7 +9997,7 @@
       </c>
       <c r="W40" s="6"/>
     </row>
-    <row r="41" spans="1:24" customFormat="1" ht="192" hidden="1">
+    <row r="41" spans="1:24" customFormat="1" ht="192">
       <c r="A41" s="58">
         <v>40</v>
       </c>
@@ -10077,7 +10062,7 @@
       <c r="V41" s="14"/>
       <c r="W41" s="6"/>
     </row>
-    <row r="42" spans="1:24" customFormat="1" ht="150" hidden="1">
+    <row r="42" spans="1:24" customFormat="1" ht="150">
       <c r="A42" s="58">
         <v>41</v>
       </c>
@@ -10144,7 +10129,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="43" spans="1:24" customFormat="1" ht="105" hidden="1">
+    <row r="43" spans="1:24" customFormat="1" ht="105">
       <c r="A43" s="58">
         <v>42</v>
       </c>
@@ -10211,7 +10196,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="44" spans="1:24" customFormat="1" ht="105" hidden="1">
+    <row r="44" spans="1:24" customFormat="1" ht="105">
       <c r="A44" s="58">
         <v>43</v>
       </c>
@@ -10278,7 +10263,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="45" spans="1:24" customFormat="1" ht="105" hidden="1">
+    <row r="45" spans="1:24" customFormat="1" ht="105">
       <c r="A45" s="58">
         <v>44</v>
       </c>
@@ -10347,7 +10332,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="46" spans="1:24" customFormat="1" ht="240" hidden="1">
+    <row r="46" spans="1:24" customFormat="1" ht="240">
       <c r="A46" s="58">
         <v>45</v>
       </c>
@@ -10412,7 +10397,7 @@
       </c>
       <c r="W46" s="67"/>
     </row>
-    <row r="47" spans="1:24" customFormat="1" ht="180" hidden="1">
+    <row r="47" spans="1:24" customFormat="1" ht="180">
       <c r="A47" s="58">
         <v>46</v>
       </c>
@@ -10479,7 +10464,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="48" spans="1:24" customFormat="1" ht="150" hidden="1">
+    <row r="48" spans="1:24" customFormat="1" ht="150">
       <c r="A48" s="58">
         <v>47</v>
       </c>
@@ -10546,7 +10531,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="49" spans="1:23" customFormat="1" ht="48" hidden="1">
+    <row r="49" spans="1:23" customFormat="1" ht="48">
       <c r="A49" s="58">
         <v>48</v>
       </c>
@@ -10611,7 +10596,7 @@
       </c>
       <c r="W49" s="6"/>
     </row>
-    <row r="50" spans="1:23" customFormat="1" ht="48" hidden="1">
+    <row r="50" spans="1:23" customFormat="1" ht="48">
       <c r="A50" s="58">
         <v>49</v>
       </c>
@@ -10678,7 +10663,7 @@
       </c>
       <c r="W50" s="69"/>
     </row>
-    <row r="51" spans="1:23" customFormat="1" ht="48" hidden="1">
+    <row r="51" spans="1:23" customFormat="1" ht="48">
       <c r="A51" s="58">
         <v>50</v>
       </c>
@@ -10745,7 +10730,7 @@
       </c>
       <c r="W51" s="9"/>
     </row>
-    <row r="52" spans="1:23" customFormat="1" ht="112" hidden="1">
+    <row r="52" spans="1:23" customFormat="1" ht="112">
       <c r="A52" s="58">
         <v>51</v>
       </c>
@@ -10814,7 +10799,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="53" spans="1:23" customFormat="1" ht="128" hidden="1">
+    <row r="53" spans="1:23" customFormat="1" ht="128">
       <c r="A53" s="58">
         <v>52</v>
       </c>
@@ -10883,7 +10868,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="54" spans="1:23" customFormat="1" ht="144" hidden="1">
+    <row r="54" spans="1:23" customFormat="1" ht="144">
       <c r="A54" s="58">
         <v>53</v>
       </c>
@@ -10952,7 +10937,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="55" spans="1:23" customFormat="1" ht="112" hidden="1">
+    <row r="55" spans="1:23" customFormat="1" ht="112">
       <c r="A55" s="58">
         <v>54</v>
       </c>
@@ -11021,7 +11006,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="56" spans="1:23" customFormat="1" ht="112" hidden="1">
+    <row r="56" spans="1:23" customFormat="1" ht="112">
       <c r="A56" s="58">
         <v>55</v>
       </c>
@@ -11090,7 +11075,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="57" spans="1:23" customFormat="1" ht="176" hidden="1">
+    <row r="57" spans="1:23" customFormat="1" ht="176">
       <c r="A57" s="58">
         <v>56</v>
       </c>
@@ -11159,7 +11144,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="58" spans="1:23" customFormat="1" ht="160" hidden="1">
+    <row r="58" spans="1:23" customFormat="1" ht="160">
       <c r="A58" s="58">
         <v>57</v>
       </c>
@@ -11226,7 +11211,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="59" spans="1:23" customFormat="1" ht="80" hidden="1">
+    <row r="59" spans="1:23" customFormat="1" ht="80">
       <c r="A59" s="58">
         <v>58</v>
       </c>
@@ -11293,7 +11278,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="60" spans="1:23" customFormat="1" ht="16" hidden="1">
+    <row r="60" spans="1:23" customFormat="1" ht="16">
       <c r="A60" s="58">
         <v>59</v>
       </c>
@@ -11358,7 +11343,7 @@
       </c>
       <c r="W60" s="6"/>
     </row>
-    <row r="61" spans="1:23" customFormat="1" ht="16" hidden="1">
+    <row r="61" spans="1:23" customFormat="1" ht="16">
       <c r="A61" s="58">
         <v>60</v>
       </c>
@@ -11492,7 +11477,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="63" spans="1:23" customFormat="1" ht="48" hidden="1">
+    <row r="63" spans="1:23" customFormat="1" ht="48">
       <c r="A63" s="58">
         <v>62</v>
       </c>
@@ -11559,7 +11544,7 @@
       </c>
       <c r="W63" s="6"/>
     </row>
-    <row r="64" spans="1:23" customFormat="1" ht="48" hidden="1">
+    <row r="64" spans="1:23" customFormat="1" ht="48">
       <c r="A64" s="58">
         <v>63</v>
       </c>
@@ -11626,7 +11611,7 @@
       </c>
       <c r="W64" s="6"/>
     </row>
-    <row r="65" spans="1:23" customFormat="1" ht="32" hidden="1">
+    <row r="65" spans="1:23" customFormat="1" ht="32">
       <c r="A65" s="58">
         <v>64</v>
       </c>
@@ -11689,7 +11674,7 @@
       <c r="V65" s="6"/>
       <c r="W65" s="6"/>
     </row>
-    <row r="66" spans="1:23" customFormat="1" ht="64" hidden="1">
+    <row r="66" spans="1:23" customFormat="1" ht="64">
       <c r="A66" s="58">
         <v>65</v>
       </c>
@@ -11752,7 +11737,7 @@
       <c r="V66" s="6"/>
       <c r="W66" s="6"/>
     </row>
-    <row r="67" spans="1:23" customFormat="1" ht="96" hidden="1">
+    <row r="67" spans="1:23" customFormat="1" ht="96">
       <c r="A67" s="58">
         <v>66</v>
       </c>
@@ -11815,7 +11800,7 @@
       <c r="V67" s="6"/>
       <c r="W67" s="6"/>
     </row>
-    <row r="68" spans="1:23" customFormat="1" ht="64" hidden="1">
+    <row r="68" spans="1:23" customFormat="1" ht="64">
       <c r="A68" s="58">
         <v>67</v>
       </c>
@@ -11878,7 +11863,7 @@
       <c r="V68" s="6"/>
       <c r="W68" s="6"/>
     </row>
-    <row r="69" spans="1:23" customFormat="1" ht="32" hidden="1">
+    <row r="69" spans="1:23" customFormat="1" ht="32">
       <c r="A69" s="58">
         <v>68</v>
       </c>
@@ -12012,7 +11997,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="71" spans="1:23" customFormat="1" ht="80" hidden="1">
+    <row r="71" spans="1:23" customFormat="1" ht="80">
       <c r="A71" s="63">
         <v>70</v>
       </c>
@@ -12077,7 +12062,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="72" spans="1:23" customFormat="1" ht="112" hidden="1">
+    <row r="72" spans="1:23" customFormat="1" ht="112">
       <c r="A72" s="58">
         <v>71</v>
       </c>
@@ -12144,7 +12129,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="73" spans="1:23" customFormat="1" ht="80" hidden="1">
+    <row r="73" spans="1:23" customFormat="1" ht="80">
       <c r="A73" s="58">
         <v>72</v>
       </c>
@@ -12207,7 +12192,7 @@
       <c r="V73" s="65"/>
       <c r="W73" s="65"/>
     </row>
-    <row r="74" spans="1:23" ht="80" hidden="1">
+    <row r="74" spans="1:23" ht="80">
       <c r="A74" s="63">
         <v>73</v>
       </c>
@@ -12274,7 +12259,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="144" hidden="1">
+    <row r="75" spans="1:23" ht="144">
       <c r="A75" s="58">
         <v>74</v>
       </c>
@@ -12343,7 +12328,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="80" hidden="1">
+    <row r="76" spans="1:23" ht="80">
       <c r="A76" s="63">
         <v>75</v>
       </c>
@@ -12408,7 +12393,7 @@
       <c r="V76" s="80"/>
       <c r="W76" s="80"/>
     </row>
-    <row r="77" spans="1:23" ht="48" hidden="1">
+    <row r="77" spans="1:23" ht="48">
       <c r="A77" s="63">
         <v>76</v>
       </c>
@@ -12471,7 +12456,7 @@
       <c r="V77" s="80"/>
       <c r="W77" s="80"/>
     </row>
-    <row r="78" spans="1:23" ht="64" hidden="1">
+    <row r="78" spans="1:23" ht="64">
       <c r="A78" s="63">
         <v>77</v>
       </c>
@@ -12536,7 +12521,7 @@
       </c>
       <c r="W78" s="80"/>
     </row>
-    <row r="79" spans="1:23" ht="48" hidden="1">
+    <row r="79" spans="1:23" ht="48">
       <c r="A79" s="58">
         <v>78</v>
       </c>
@@ -12603,7 +12588,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="32" hidden="1">
+    <row r="80" spans="1:23" ht="32">
       <c r="A80" s="96">
         <v>79</v>
       </c>
@@ -12668,7 +12653,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="32" hidden="1">
+    <row r="81" spans="1:23" ht="32">
       <c r="A81" s="63">
         <v>80</v>
       </c>
@@ -12731,7 +12716,7 @@
       <c r="V81" s="80"/>
       <c r="W81" s="80"/>
     </row>
-    <row r="82" spans="1:23" ht="32" hidden="1">
+    <row r="82" spans="1:23" ht="32">
       <c r="A82" s="58">
         <v>81</v>
       </c>
@@ -12794,7 +12779,7 @@
       <c r="V82" s="80"/>
       <c r="W82" s="80"/>
     </row>
-    <row r="83" spans="1:23" ht="144" hidden="1">
+    <row r="83" spans="1:23" ht="144">
       <c r="A83" s="63">
         <v>82</v>
       </c>
@@ -12863,7 +12848,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="80" hidden="1">
+    <row r="84" spans="1:23" ht="80">
       <c r="A84" s="63">
         <v>83</v>
       </c>
@@ -13135,7 +13120,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="80" hidden="1">
+    <row r="88" spans="1:23" ht="80">
       <c r="A88" s="63">
         <v>87</v>
       </c>
@@ -13204,7 +13189,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="64" hidden="1">
+    <row r="89" spans="1:23" ht="64">
       <c r="A89" s="63">
         <v>88</v>
       </c>
@@ -13247,7 +13232,7 @@
       </c>
       <c r="W89" s="69"/>
     </row>
-    <row r="90" spans="1:23" ht="48" hidden="1">
+    <row r="90" spans="1:23" ht="48">
       <c r="A90" s="58">
         <v>89</v>
       </c>
@@ -13292,7 +13277,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="48" hidden="1">
+    <row r="91" spans="1:23" ht="48">
       <c r="A91" s="63">
         <v>90</v>
       </c>
@@ -13337,7 +13322,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="64" hidden="1">
+    <row r="92" spans="1:23" ht="64">
       <c r="A92" s="63">
         <v>91</v>
       </c>
@@ -13473,7 +13458,7 @@
       </c>
       <c r="W93" s="69"/>
     </row>
-    <row r="94" spans="1:23" ht="32" hidden="1">
+    <row r="94" spans="1:23" ht="32">
       <c r="A94" s="58">
         <v>93</v>
       </c>
@@ -13603,7 +13588,7 @@
       </c>
       <c r="W95" s="69"/>
     </row>
-    <row r="96" spans="1:23" ht="32" hidden="1">
+    <row r="96" spans="1:23" ht="32">
       <c r="A96" s="58">
         <v>95</v>
       </c>
@@ -13733,7 +13718,7 @@
       </c>
       <c r="W97" s="69"/>
     </row>
-    <row r="98" spans="1:23" ht="32" hidden="1">
+    <row r="98" spans="1:23" ht="32">
       <c r="A98" s="58">
         <v>97</v>
       </c>
@@ -13796,7 +13781,7 @@
       </c>
       <c r="W98" s="69"/>
     </row>
-    <row r="99" spans="1:23" ht="96" hidden="1">
+    <row r="99" spans="1:23" ht="96">
       <c r="A99" s="63">
         <v>98</v>
       </c>
@@ -13863,7 +13848,7 @@
       </c>
       <c r="W99" s="80"/>
     </row>
-    <row r="100" spans="1:23" ht="80" hidden="1">
+    <row r="100" spans="1:23" ht="80">
       <c r="A100" s="63">
         <v>99</v>
       </c>
@@ -14139,7 +14124,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="80" hidden="1">
+    <row r="104" spans="1:23" ht="80">
       <c r="A104" s="58">
         <v>103</v>
       </c>
@@ -14239,8 +14224,8 @@
       <c r="J105" s="80" t="s">
         <v>696</v>
       </c>
-      <c r="K105" s="110" t="s">
-        <v>854</v>
+      <c r="K105" s="80" t="s">
+        <v>855</v>
       </c>
       <c r="L105" s="98">
         <v>29290</v>
@@ -14308,7 +14293,9 @@
       <c r="J106" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="K106" s="80"/>
+      <c r="K106" s="80" t="s">
+        <v>854</v>
+      </c>
       <c r="L106" s="80" t="s">
         <v>105</v>
       </c>
@@ -14683,7 +14670,7 @@
       </c>
       <c r="W111" s="80"/>
     </row>
-    <row r="112" spans="1:23" ht="80" hidden="1">
+    <row r="112" spans="1:23" ht="80">
       <c r="A112" s="58">
         <v>108</v>
       </c>
@@ -14986,7 +14973,9 @@
       <c r="J116" s="80" t="s">
         <v>808</v>
       </c>
-      <c r="K116" s="80"/>
+      <c r="K116" s="80" t="s">
+        <v>845</v>
+      </c>
       <c r="L116" s="80" t="s">
         <v>180</v>
       </c>
@@ -15055,7 +15044,9 @@
       <c r="J117" s="80" t="s">
         <v>809</v>
       </c>
-      <c r="K117" s="80"/>
+      <c r="K117" s="80" t="s">
+        <v>845</v>
+      </c>
       <c r="L117" s="80" t="s">
         <v>798</v>
       </c>
@@ -15093,7 +15084,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="176" hidden="1">
+    <row r="118" spans="1:23" ht="176">
       <c r="A118" s="63">
         <v>114</v>
       </c>
@@ -15454,7 +15445,7 @@
       <c r="B2" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="110" t="s">
         <v>553</v>
       </c>
       <c r="K2" s="21">
@@ -15600,7 +15591,7 @@
       <c r="B3" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="D3" s="112"/>
+      <c r="D3" s="111"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="K3" s="17">
@@ -15785,7 +15776,7 @@
       </c>
     </row>
     <row r="4" spans="1:56">
-      <c r="D4" s="112"/>
+      <c r="D4" s="111"/>
       <c r="K4" s="17" t="e">
         <f t="shared" ref="K4:BC4" si="40">_xlfn.XLOOKUP(K3,$A$15:$A$17,$B$15:$B$17)</f>
         <v>#N/A</v>
@@ -15968,7 +15959,7 @@
       </c>
     </row>
     <row r="5" spans="1:56">
-      <c r="D5" s="112"/>
+      <c r="D5" s="111"/>
       <c r="G5"/>
       <c r="K5" s="17">
         <f t="shared" ref="K5:BC5" si="41">DAY(K2)</f>
@@ -16152,7 +16143,7 @@
       </c>
     </row>
     <row r="6" spans="1:56">
-      <c r="D6" s="112"/>
+      <c r="D6" s="111"/>
       <c r="K6" s="17" t="s">
         <v>555</v>
       </c>
@@ -16290,11 +16281,11 @@
       </c>
     </row>
     <row r="7" spans="1:56" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D7" s="112"/>
+      <c r="D7" s="111"/>
       <c r="AH7" s="27"/>
     </row>
     <row r="8" spans="1:56" ht="17" thickBot="1">
-      <c r="D8" s="112"/>
+      <c r="D8" s="111"/>
       <c r="F8" s="24" t="s">
         <v>562</v>
       </c>
@@ -16352,7 +16343,7 @@
       <c r="BD8" s="30"/>
     </row>
     <row r="9" spans="1:56" ht="16" thickBot="1">
-      <c r="D9" s="112"/>
+      <c r="D9" s="111"/>
       <c r="I9" s="27"/>
       <c r="N9" s="36"/>
       <c r="S9" s="37"/>
@@ -16375,7 +16366,7 @@
       <c r="BD9" s="36"/>
     </row>
     <row r="10" spans="1:56" ht="33" thickBot="1">
-      <c r="D10" s="112"/>
+      <c r="D10" s="111"/>
       <c r="F10" s="24" t="s">
         <v>565</v>
       </c>
@@ -16433,7 +16424,7 @@
       <c r="BD10" s="42"/>
     </row>
     <row r="11" spans="1:56" ht="16" thickBot="1">
-      <c r="D11" s="112"/>
+      <c r="D11" s="111"/>
       <c r="G11"/>
       <c r="I11" s="27"/>
       <c r="AB11" s="2"/>
@@ -16448,7 +16439,7 @@
       <c r="BC11" s="17"/>
     </row>
     <row r="12" spans="1:56" ht="16" thickBot="1">
-      <c r="D12" s="112"/>
+      <c r="D12" s="111"/>
       <c r="G12"/>
       <c r="I12" s="39" t="s">
         <v>568</v>
@@ -16501,12 +16492,12 @@
       <c r="BD12" s="42"/>
     </row>
     <row r="13" spans="1:56" ht="16" thickBot="1">
-      <c r="D13" s="112"/>
+      <c r="D13" s="111"/>
       <c r="G13"/>
       <c r="I13" s="27"/>
     </row>
     <row r="14" spans="1:56" ht="16" thickBot="1">
-      <c r="D14" s="112"/>
+      <c r="D14" s="111"/>
       <c r="G14"/>
       <c r="I14" s="47" t="s">
         <v>569</v>
@@ -16594,12 +16585,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16768,15 +16756,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91500E67-CFBD-4E57-93CA-25297AD67667}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6ECE83-F240-478D-BE60-3B98A1630AA1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16801,10 +16793,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6ECE83-F240-478D-BE60-3B98A1630AA1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91500E67-CFBD-4E57-93CA-25297AD67667}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
JADE-1691 latest mapping changes
</commit_message>
<xml_diff>
--- a/mapping/docs/Tracking DEMS Integration Data Mapping v1.20.xlsx
+++ b/mapping/docs/Tracking DEMS Integration Data Mapping v1.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/git/jade/jpss-jade-ccm/mapping/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916E531A-5E82-764A-93A4-D530B479522F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576355BB-6B8A-A84B-A9F5-20E33614361C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2574" uniqueCount="856">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2581" uniqueCount="859">
   <si>
     <t>Change Date</t>
   </si>
@@ -4030,16 +4030,25 @@
     <t>Updated mapping (display name is made of concatenated names)</t>
   </si>
   <si>
-    <t>QUESTION: Not updated; what about the existing logic to upper case the last name of each accused (last name, first name)</t>
-  </si>
-  <si>
-    <t>QUESTION: Not updated; this implies use of concatenated names instead of MAPID 23</t>
-  </si>
-  <si>
-    <t>Always associate an accused to a case with ParticipantType = "Accused"</t>
-  </si>
-  <si>
     <t>Already done.  Previous issues with DEMS API</t>
+  </si>
+  <si>
+    <t>QUESTION: Not updated; what about the existing logic to upper case the last name of each accused (last name, first name) -- commented in BCPSDEMS-530</t>
+  </si>
+  <si>
+    <t>QUESTION: Not updated; this implies use of concatenated names instead of MAPID 23.  Also, the custom field "Full Name and Birth" does not exist -- commented in BCPSDEMS-530</t>
+  </si>
+  <si>
+    <t>Response: Always associate an accused to a case with ParticipantType = "Accused"</t>
+  </si>
+  <si>
+    <t>Response: Always defaults to type = "Individual" when creating a participant (Person) in DEMS</t>
+  </si>
+  <si>
+    <t>Response: Do nothing</t>
+  </si>
+  <si>
+    <t>QUESTION: Cannot complete mapping; "Court File Details" does not exist</t>
   </si>
 </sst>
 </file>
@@ -4519,7 +4528,7 @@
     <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4856,6 +4865,9 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="6" builtinId="30"/>
@@ -4867,7 +4879,15 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="36">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -6273,50 +6293,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1ED591A2-D5F5-48E8-9A56-F77B33C2B10C}" name="Table4" displayName="Table4" ref="A1:F18" totalsRowShown="0" headerRowDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1ED591A2-D5F5-48E8-9A56-F77B33C2B10C}" name="Table4" displayName="Table4" ref="A1:F18" totalsRowShown="0" headerRowDxfId="35">
   <autoFilter ref="A1:F18" xr:uid="{1ED591A2-D5F5-48E8-9A56-F77B33C2B10C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F18">
     <sortCondition ref="A1:A18"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="6" xr3:uid="{5D50D0B9-8A1C-41DB-91A1-91EACB043682}" name="Priority Level" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{F08A0110-EDC5-430B-8AB7-7A180EC1B45C}" name="Scenario" dataDxfId="32"/>
-    <tableColumn id="1" xr3:uid="{398E92A7-526C-4756-A29B-B4B25D12F1F4}" name="Integration Pattern" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{40EC0948-6F7E-4FEC-838A-39FCF8417022}" name="Event" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{728856FA-075A-4E50-B7C4-D656511364D9}" name="Data Fields / Report" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{8F7E9398-7640-4FAB-892D-F1CAF1397848}" name="Note" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{5D50D0B9-8A1C-41DB-91A1-91EACB043682}" name="Priority Level" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{F08A0110-EDC5-430B-8AB7-7A180EC1B45C}" name="Scenario" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{398E92A7-526C-4756-A29B-B4B25D12F1F4}" name="Integration Pattern" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{40EC0948-6F7E-4FEC-838A-39FCF8417022}" name="Event" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{728856FA-075A-4E50-B7C4-D656511364D9}" name="Data Fields / Report" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{8F7E9398-7640-4FAB-892D-F1CAF1397848}" name="Note" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A292DBCF-B35F-4E38-91EC-93A3024A386F}" name="Table2" displayName="Table2" ref="A1:W121" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23" headerRowCellStyle="Good">
-  <autoFilter ref="A1:W121" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A292DBCF-B35F-4E38-91EC-93A3024A386F}" name="Table2" displayName="Table2" ref="A1:W121" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24" headerRowCellStyle="Good">
+  <autoFilter ref="A1:W121" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="10">
+      <colorFilter dxfId="0" cellColor="0"/>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{835DEB9C-EF50-49F3-AADC-8EEC259AD441}" name="#" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{8E79AED4-9838-4FD0-9B84-9FCF2119C980}" name="Status" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{A4589D1E-D2D1-4CEC-B6FA-6090826F1D45}" name="Scenario ID" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{40563DC3-C720-4025-8178-BBB7E36F5A72}" name="Scenario Name" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{CEA1207D-90E6-4713-9B1D-FDF532A800C8}" name="Last Updated" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{CA0626E0-56F3-42D4-9D46-C866C1128CB3}" name="JUSTIN Field #" dataDxfId="17"/>
-    <tableColumn id="21" xr3:uid="{75D98204-8E7B-4EFE-BAB5-48B68ECEB743}" name="JUSTIN Source" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{3ADDC782-0076-436D-B6D9-3F61F3C19AAF}" name="JUSTIN Data Element" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{E8B7DD64-48AC-4CA5-A297-D08EA732EB76}" name="JUSTIN Data Label" dataDxfId="14"/>
-    <tableColumn id="9" xr3:uid="{5BC3FDBB-2BD9-46CD-8A3F-9938767E0B66}" name="JUSTIN Data Description" dataDxfId="13"/>
-    <tableColumn id="23" xr3:uid="{4B011560-A692-3A46-B05D-74E45C8CEF54}" name="Tracking" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{11ECEB32-CAB5-4C86-B58D-C17D16FBAA1F}" name="JUSTIN Sample Data" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{D09AB9DD-52FF-4DF7-AE25-0D694B6F01B1}" name="JUSTIN to Common Mapping Rules" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{D4AE8E14-6396-41D2-BC89-18DD52849BE2}" name="JUSTIN to Common Mapping Sample Data" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{B4F6F913-B7DE-4BA0-B52D-31728062A38D}" name="Common Data Element" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{C34386F3-CD56-407B-BA5A-3C9C19CFC499}" name="Common Data Type" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{E9F54F19-D5FE-4557-A6B7-9D5B084EC9A9}" name="Common to DEMS Mapping Rules" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{EA92266D-452D-45AF-B0EB-C90A4219660F}" name="Common to DEMS Mapping  Sample Data" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{50F4E4ED-21B9-4476-9E2E-5A978C219888}" name="DEMS Data Element" dataDxfId="4"/>
-    <tableColumn id="22" xr3:uid="{CDC2C70F-F494-4B60-A113-6BA8074AFB61}" name="DEMS Data Element Type" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{56EB14F6-1C9B-4B5C-B520-7C2B782FD072}" name="Business Value or Decision" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{439A6CB0-3E94-459D-94D4-B0E6CDAF1070}" name="Priority (MoSCoW)" dataDxfId="1"/>
-    <tableColumn id="20" xr3:uid="{B9BF0D1A-DA40-43A3-A56B-2B0D1933177B}" name="Additional Details" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{835DEB9C-EF50-49F3-AADC-8EEC259AD441}" name="#" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{8E79AED4-9838-4FD0-9B84-9FCF2119C980}" name="Status" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{A4589D1E-D2D1-4CEC-B6FA-6090826F1D45}" name="Scenario ID" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{40563DC3-C720-4025-8178-BBB7E36F5A72}" name="Scenario Name" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{CEA1207D-90E6-4713-9B1D-FDF532A800C8}" name="Last Updated" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{CA0626E0-56F3-42D4-9D46-C866C1128CB3}" name="JUSTIN Field #" dataDxfId="18"/>
+    <tableColumn id="21" xr3:uid="{75D98204-8E7B-4EFE-BAB5-48B68ECEB743}" name="JUSTIN Source" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{3ADDC782-0076-436D-B6D9-3F61F3C19AAF}" name="JUSTIN Data Element" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{E8B7DD64-48AC-4CA5-A297-D08EA732EB76}" name="JUSTIN Data Label" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{5BC3FDBB-2BD9-46CD-8A3F-9938767E0B66}" name="JUSTIN Data Description" dataDxfId="14"/>
+    <tableColumn id="23" xr3:uid="{4B011560-A692-3A46-B05D-74E45C8CEF54}" name="Tracking" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{11ECEB32-CAB5-4C86-B58D-C17D16FBAA1F}" name="JUSTIN Sample Data" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{D09AB9DD-52FF-4DF7-AE25-0D694B6F01B1}" name="JUSTIN to Common Mapping Rules" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{D4AE8E14-6396-41D2-BC89-18DD52849BE2}" name="JUSTIN to Common Mapping Sample Data" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{B4F6F913-B7DE-4BA0-B52D-31728062A38D}" name="Common Data Element" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{C34386F3-CD56-407B-BA5A-3C9C19CFC499}" name="Common Data Type" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{E9F54F19-D5FE-4557-A6B7-9D5B084EC9A9}" name="Common to DEMS Mapping Rules" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{EA92266D-452D-45AF-B0EB-C90A4219660F}" name="Common to DEMS Mapping  Sample Data" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{50F4E4ED-21B9-4476-9E2E-5A978C219888}" name="DEMS Data Element" dataDxfId="5"/>
+    <tableColumn id="22" xr3:uid="{CDC2C70F-F494-4B60-A113-6BA8074AFB61}" name="DEMS Data Element Type" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{56EB14F6-1C9B-4B5C-B520-7C2B782FD072}" name="Business Value or Decision" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{439A6CB0-3E94-459D-94D4-B0E6CDAF1070}" name="Priority (MoSCoW)" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{B9BF0D1A-DA40-43A3-A56B-2B0D1933177B}" name="Additional Details" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7281,10 +7305,10 @@
   <dimension ref="A1:X121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="O112" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="J102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O114" sqref="O114"/>
+      <selection pane="bottomRight" activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.5" defaultRowHeight="15"/>
@@ -7384,7 +7408,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:23" customFormat="1" ht="48">
+    <row r="2" spans="1:23" customFormat="1" ht="48" hidden="1">
       <c r="A2" s="58">
         <v>1</v>
       </c>
@@ -7449,7 +7473,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="3" spans="1:23" customFormat="1" ht="256">
+    <row r="3" spans="1:23" customFormat="1" ht="256" hidden="1">
       <c r="A3" s="58">
         <v>2</v>
       </c>
@@ -7520,7 +7544,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="4" spans="1:23" customFormat="1" ht="80">
+    <row r="4" spans="1:23" customFormat="1" ht="80" hidden="1">
       <c r="A4" s="58">
         <v>3</v>
       </c>
@@ -7575,7 +7599,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:23" customFormat="1" ht="16">
+    <row r="5" spans="1:23" customFormat="1" ht="16" hidden="1">
       <c r="A5" s="58">
         <v>4</v>
       </c>
@@ -7626,7 +7650,7 @@
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:23" customFormat="1" ht="272">
+    <row r="6" spans="1:23" customFormat="1" ht="272" hidden="1">
       <c r="A6" s="58">
         <v>5</v>
       </c>
@@ -7695,7 +7719,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:23" customFormat="1" ht="256">
+    <row r="7" spans="1:23" customFormat="1" ht="256" hidden="1">
       <c r="A7" s="58">
         <v>6</v>
       </c>
@@ -7764,7 +7788,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:23" customFormat="1" ht="128">
+    <row r="8" spans="1:23" customFormat="1" ht="128" hidden="1">
       <c r="A8" s="58">
         <v>7</v>
       </c>
@@ -7833,7 +7857,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="112">
+    <row r="9" spans="1:23" ht="112" hidden="1">
       <c r="A9" s="58">
         <v>8</v>
       </c>
@@ -7902,7 +7926,7 @@
       </c>
       <c r="W9" s="6"/>
     </row>
-    <row r="10" spans="1:23" ht="32">
+    <row r="10" spans="1:23" ht="32" hidden="1">
       <c r="A10" s="58">
         <v>9</v>
       </c>
@@ -7969,7 +7993,7 @@
       </c>
       <c r="W10" s="6"/>
     </row>
-    <row r="11" spans="1:23" ht="32">
+    <row r="11" spans="1:23" ht="32" hidden="1">
       <c r="A11" s="58">
         <v>10</v>
       </c>
@@ -8036,7 +8060,7 @@
       </c>
       <c r="W11" s="6"/>
     </row>
-    <row r="12" spans="1:23" ht="96">
+    <row r="12" spans="1:23" ht="96" hidden="1">
       <c r="A12" s="58">
         <v>11</v>
       </c>
@@ -8103,7 +8127,7 @@
       </c>
       <c r="W12" s="6"/>
     </row>
-    <row r="13" spans="1:23" ht="128">
+    <row r="13" spans="1:23" ht="128" hidden="1">
       <c r="A13" s="84">
         <v>12</v>
       </c>
@@ -8172,7 +8196,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="14" spans="1:23" customFormat="1" ht="128">
+    <row r="14" spans="1:23" customFormat="1" ht="128" hidden="1">
       <c r="A14" s="84">
         <v>13</v>
       </c>
@@ -8241,7 +8265,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="15" spans="1:23" customFormat="1" ht="32">
+    <row r="15" spans="1:23" customFormat="1" ht="32" hidden="1">
       <c r="A15" s="58">
         <v>14</v>
       </c>
@@ -8306,7 +8330,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="160">
+    <row r="16" spans="1:23" ht="160" hidden="1">
       <c r="A16" s="58">
         <v>15</v>
       </c>
@@ -8377,7 +8401,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="17" spans="1:23" customFormat="1" ht="80">
+    <row r="17" spans="1:23" customFormat="1" ht="80" hidden="1">
       <c r="A17" s="58">
         <v>16</v>
       </c>
@@ -8444,7 +8468,7 @@
       </c>
       <c r="W17" s="6"/>
     </row>
-    <row r="18" spans="1:23" customFormat="1" ht="144">
+    <row r="18" spans="1:23" customFormat="1" ht="144" hidden="1">
       <c r="A18" s="58">
         <v>17</v>
       </c>
@@ -8511,7 +8535,7 @@
       </c>
       <c r="W18" s="59"/>
     </row>
-    <row r="19" spans="1:23" customFormat="1" ht="112">
+    <row r="19" spans="1:23" customFormat="1" ht="112" hidden="1">
       <c r="A19" s="58">
         <v>18</v>
       </c>
@@ -8578,7 +8602,7 @@
       </c>
       <c r="W19" s="6"/>
     </row>
-    <row r="20" spans="1:23" customFormat="1" ht="288">
+    <row r="20" spans="1:23" customFormat="1" ht="288" hidden="1">
       <c r="A20" s="58">
         <v>19</v>
       </c>
@@ -8647,7 +8671,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:23" customFormat="1" ht="335">
+    <row r="21" spans="1:23" customFormat="1" ht="335" hidden="1">
       <c r="A21" s="58">
         <v>20</v>
       </c>
@@ -8716,7 +8740,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="22" spans="1:23" customFormat="1" ht="96">
+    <row r="22" spans="1:23" customFormat="1" ht="96" hidden="1">
       <c r="A22" s="58">
         <v>21</v>
       </c>
@@ -8781,7 +8805,7 @@
       </c>
       <c r="W22" s="9"/>
     </row>
-    <row r="23" spans="1:23" customFormat="1" ht="80">
+    <row r="23" spans="1:23" customFormat="1" ht="80" hidden="1">
       <c r="A23" s="63">
         <v>22</v>
       </c>
@@ -8850,7 +8874,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="24" spans="1:23" s="6" customFormat="1" ht="80">
+    <row r="24" spans="1:23" s="6" customFormat="1" ht="80" hidden="1">
       <c r="A24" s="58">
         <v>23</v>
       </c>
@@ -8915,7 +8939,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="25" spans="1:23" customFormat="1" ht="256">
+    <row r="25" spans="1:23" customFormat="1" ht="256" hidden="1">
       <c r="A25" s="93">
         <v>24</v>
       </c>
@@ -8984,7 +9008,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="26" spans="1:23" customFormat="1" ht="80">
+    <row r="26" spans="1:23" customFormat="1" ht="80" hidden="1">
       <c r="A26" s="58">
         <v>25</v>
       </c>
@@ -9050,7 +9074,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:23" customFormat="1" ht="256">
+    <row r="27" spans="1:23" customFormat="1" ht="256" hidden="1">
       <c r="A27" s="58">
         <v>26</v>
       </c>
@@ -9117,7 +9141,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="28" spans="1:23" customFormat="1" ht="96">
+    <row r="28" spans="1:23" customFormat="1" ht="96" hidden="1">
       <c r="A28" s="84">
         <v>27</v>
       </c>
@@ -9186,7 +9210,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="29" spans="1:23" customFormat="1" ht="32">
+    <row r="29" spans="1:23" customFormat="1" ht="32" hidden="1">
       <c r="A29" s="63">
         <v>28</v>
       </c>
@@ -9249,7 +9273,7 @@
       <c r="V29" s="6"/>
       <c r="W29" s="9"/>
     </row>
-    <row r="30" spans="1:23" customFormat="1" ht="48">
+    <row r="30" spans="1:23" customFormat="1" ht="48" hidden="1">
       <c r="A30" s="95">
         <v>29</v>
       </c>
@@ -9318,7 +9342,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="31" spans="1:23" customFormat="1" ht="128">
+    <row r="31" spans="1:23" customFormat="1" ht="128" hidden="1">
       <c r="A31" s="93">
         <v>30</v>
       </c>
@@ -9387,7 +9411,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="1:23" customFormat="1" ht="208">
+    <row r="32" spans="1:23" customFormat="1" ht="208" hidden="1">
       <c r="A32" s="58">
         <v>31</v>
       </c>
@@ -9452,7 +9476,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="33" spans="1:24" s="6" customFormat="1" ht="192">
+    <row r="33" spans="1:24" s="6" customFormat="1" ht="192" hidden="1">
       <c r="A33" s="58">
         <v>32</v>
       </c>
@@ -9522,7 +9546,7 @@
       </c>
       <c r="X33" s="90"/>
     </row>
-    <row r="34" spans="1:24" customFormat="1" ht="112">
+    <row r="34" spans="1:24" customFormat="1" ht="112" hidden="1">
       <c r="A34" s="58">
         <v>33</v>
       </c>
@@ -9591,7 +9615,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="35" spans="1:24" customFormat="1" ht="176">
+    <row r="35" spans="1:24" customFormat="1" ht="176" hidden="1">
       <c r="A35" s="58">
         <v>34</v>
       </c>
@@ -9660,7 +9684,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="36" spans="1:24" customFormat="1" ht="112">
+    <row r="36" spans="1:24" customFormat="1" ht="112" hidden="1">
       <c r="A36" s="58">
         <v>35</v>
       </c>
@@ -9727,7 +9751,7 @@
       </c>
       <c r="W36" s="6"/>
     </row>
-    <row r="37" spans="1:24" customFormat="1" ht="160">
+    <row r="37" spans="1:24" customFormat="1" ht="160" hidden="1">
       <c r="A37" s="58">
         <v>36</v>
       </c>
@@ -9794,7 +9818,7 @@
       </c>
       <c r="W37" s="6"/>
     </row>
-    <row r="38" spans="1:24" customFormat="1" ht="32">
+    <row r="38" spans="1:24" customFormat="1" ht="32" hidden="1">
       <c r="A38" s="58">
         <v>37</v>
       </c>
@@ -9861,7 +9885,7 @@
       </c>
       <c r="W38" s="6"/>
     </row>
-    <row r="39" spans="1:24" customFormat="1" ht="356">
+    <row r="39" spans="1:24" customFormat="1" ht="356" hidden="1">
       <c r="A39" s="58">
         <v>38</v>
       </c>
@@ -9930,7 +9954,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="40" spans="1:24" customFormat="1" ht="240">
+    <row r="40" spans="1:24" customFormat="1" ht="240" hidden="1">
       <c r="A40" s="58">
         <v>39</v>
       </c>
@@ -9997,7 +10021,7 @@
       </c>
       <c r="W40" s="6"/>
     </row>
-    <row r="41" spans="1:24" customFormat="1" ht="192">
+    <row r="41" spans="1:24" customFormat="1" ht="192" hidden="1">
       <c r="A41" s="58">
         <v>40</v>
       </c>
@@ -10062,7 +10086,7 @@
       <c r="V41" s="14"/>
       <c r="W41" s="6"/>
     </row>
-    <row r="42" spans="1:24" customFormat="1" ht="150">
+    <row r="42" spans="1:24" customFormat="1" ht="150" hidden="1">
       <c r="A42" s="58">
         <v>41</v>
       </c>
@@ -10129,7 +10153,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="43" spans="1:24" customFormat="1" ht="105">
+    <row r="43" spans="1:24" customFormat="1" ht="105" hidden="1">
       <c r="A43" s="58">
         <v>42</v>
       </c>
@@ -10196,7 +10220,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="44" spans="1:24" customFormat="1" ht="105">
+    <row r="44" spans="1:24" customFormat="1" ht="105" hidden="1">
       <c r="A44" s="58">
         <v>43</v>
       </c>
@@ -10263,7 +10287,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="45" spans="1:24" customFormat="1" ht="105">
+    <row r="45" spans="1:24" customFormat="1" ht="105" hidden="1">
       <c r="A45" s="58">
         <v>44</v>
       </c>
@@ -10332,7 +10356,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="46" spans="1:24" customFormat="1" ht="240">
+    <row r="46" spans="1:24" customFormat="1" ht="240" hidden="1">
       <c r="A46" s="58">
         <v>45</v>
       </c>
@@ -10397,7 +10421,7 @@
       </c>
       <c r="W46" s="67"/>
     </row>
-    <row r="47" spans="1:24" customFormat="1" ht="180">
+    <row r="47" spans="1:24" customFormat="1" ht="180" hidden="1">
       <c r="A47" s="58">
         <v>46</v>
       </c>
@@ -10464,7 +10488,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="48" spans="1:24" customFormat="1" ht="150">
+    <row r="48" spans="1:24" customFormat="1" ht="150" hidden="1">
       <c r="A48" s="58">
         <v>47</v>
       </c>
@@ -10531,7 +10555,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="49" spans="1:23" customFormat="1" ht="48">
+    <row r="49" spans="1:23" customFormat="1" ht="48" hidden="1">
       <c r="A49" s="58">
         <v>48</v>
       </c>
@@ -10596,7 +10620,7 @@
       </c>
       <c r="W49" s="6"/>
     </row>
-    <row r="50" spans="1:23" customFormat="1" ht="48">
+    <row r="50" spans="1:23" customFormat="1" ht="48" hidden="1">
       <c r="A50" s="58">
         <v>49</v>
       </c>
@@ -10663,7 +10687,7 @@
       </c>
       <c r="W50" s="69"/>
     </row>
-    <row r="51" spans="1:23" customFormat="1" ht="48">
+    <row r="51" spans="1:23" customFormat="1" ht="48" hidden="1">
       <c r="A51" s="58">
         <v>50</v>
       </c>
@@ -10730,7 +10754,7 @@
       </c>
       <c r="W51" s="9"/>
     </row>
-    <row r="52" spans="1:23" customFormat="1" ht="112">
+    <row r="52" spans="1:23" customFormat="1" ht="112" hidden="1">
       <c r="A52" s="58">
         <v>51</v>
       </c>
@@ -10799,7 +10823,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="53" spans="1:23" customFormat="1" ht="128">
+    <row r="53" spans="1:23" customFormat="1" ht="128" hidden="1">
       <c r="A53" s="58">
         <v>52</v>
       </c>
@@ -10868,7 +10892,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="54" spans="1:23" customFormat="1" ht="144">
+    <row r="54" spans="1:23" customFormat="1" ht="144" hidden="1">
       <c r="A54" s="58">
         <v>53</v>
       </c>
@@ -10937,7 +10961,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="55" spans="1:23" customFormat="1" ht="112">
+    <row r="55" spans="1:23" customFormat="1" ht="112" hidden="1">
       <c r="A55" s="58">
         <v>54</v>
       </c>
@@ -11006,7 +11030,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="56" spans="1:23" customFormat="1" ht="112">
+    <row r="56" spans="1:23" customFormat="1" ht="112" hidden="1">
       <c r="A56" s="58">
         <v>55</v>
       </c>
@@ -11075,7 +11099,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="57" spans="1:23" customFormat="1" ht="176">
+    <row r="57" spans="1:23" customFormat="1" ht="176" hidden="1">
       <c r="A57" s="58">
         <v>56</v>
       </c>
@@ -11144,7 +11168,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="58" spans="1:23" customFormat="1" ht="160">
+    <row r="58" spans="1:23" customFormat="1" ht="160" hidden="1">
       <c r="A58" s="58">
         <v>57</v>
       </c>
@@ -11211,7 +11235,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="59" spans="1:23" customFormat="1" ht="80">
+    <row r="59" spans="1:23" customFormat="1" ht="80" hidden="1">
       <c r="A59" s="58">
         <v>58</v>
       </c>
@@ -11278,7 +11302,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="60" spans="1:23" customFormat="1" ht="16">
+    <row r="60" spans="1:23" customFormat="1" ht="16" hidden="1">
       <c r="A60" s="58">
         <v>59</v>
       </c>
@@ -11343,7 +11367,7 @@
       </c>
       <c r="W60" s="6"/>
     </row>
-    <row r="61" spans="1:23" customFormat="1" ht="16">
+    <row r="61" spans="1:23" customFormat="1" ht="16" hidden="1">
       <c r="A61" s="58">
         <v>60</v>
       </c>
@@ -11408,7 +11432,7 @@
       </c>
       <c r="W61" s="6"/>
     </row>
-    <row r="62" spans="1:23" customFormat="1" ht="32">
+    <row r="62" spans="1:23" customFormat="1" ht="32" hidden="1">
       <c r="A62" s="58">
         <v>61</v>
       </c>
@@ -11477,7 +11501,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="63" spans="1:23" customFormat="1" ht="48">
+    <row r="63" spans="1:23" customFormat="1" ht="48" hidden="1">
       <c r="A63" s="58">
         <v>62</v>
       </c>
@@ -11544,7 +11568,7 @@
       </c>
       <c r="W63" s="6"/>
     </row>
-    <row r="64" spans="1:23" customFormat="1" ht="48">
+    <row r="64" spans="1:23" customFormat="1" ht="48" hidden="1">
       <c r="A64" s="58">
         <v>63</v>
       </c>
@@ -11611,7 +11635,7 @@
       </c>
       <c r="W64" s="6"/>
     </row>
-    <row r="65" spans="1:23" customFormat="1" ht="32">
+    <row r="65" spans="1:23" customFormat="1" ht="32" hidden="1">
       <c r="A65" s="58">
         <v>64</v>
       </c>
@@ -11674,7 +11698,7 @@
       <c r="V65" s="6"/>
       <c r="W65" s="6"/>
     </row>
-    <row r="66" spans="1:23" customFormat="1" ht="64">
+    <row r="66" spans="1:23" customFormat="1" ht="64" hidden="1">
       <c r="A66" s="58">
         <v>65</v>
       </c>
@@ -11737,7 +11761,7 @@
       <c r="V66" s="6"/>
       <c r="W66" s="6"/>
     </row>
-    <row r="67" spans="1:23" customFormat="1" ht="96">
+    <row r="67" spans="1:23" customFormat="1" ht="96" hidden="1">
       <c r="A67" s="58">
         <v>66</v>
       </c>
@@ -11800,7 +11824,7 @@
       <c r="V67" s="6"/>
       <c r="W67" s="6"/>
     </row>
-    <row r="68" spans="1:23" customFormat="1" ht="64">
+    <row r="68" spans="1:23" customFormat="1" ht="64" hidden="1">
       <c r="A68" s="58">
         <v>67</v>
       </c>
@@ -11863,7 +11887,7 @@
       <c r="V68" s="6"/>
       <c r="W68" s="6"/>
     </row>
-    <row r="69" spans="1:23" customFormat="1" ht="32">
+    <row r="69" spans="1:23" customFormat="1" ht="32" hidden="1">
       <c r="A69" s="58">
         <v>68</v>
       </c>
@@ -11926,7 +11950,7 @@
       <c r="V69" s="6"/>
       <c r="W69" s="6"/>
     </row>
-    <row r="70" spans="1:23" customFormat="1" ht="208">
+    <row r="70" spans="1:23" customFormat="1" ht="208" hidden="1">
       <c r="A70" s="58">
         <v>69</v>
       </c>
@@ -11997,7 +12021,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="71" spans="1:23" customFormat="1" ht="80">
+    <row r="71" spans="1:23" customFormat="1" ht="80" hidden="1">
       <c r="A71" s="63">
         <v>70</v>
       </c>
@@ -12062,7 +12086,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="72" spans="1:23" customFormat="1" ht="112">
+    <row r="72" spans="1:23" customFormat="1" ht="112" hidden="1">
       <c r="A72" s="58">
         <v>71</v>
       </c>
@@ -12129,7 +12153,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="73" spans="1:23" customFormat="1" ht="80">
+    <row r="73" spans="1:23" customFormat="1" ht="80" hidden="1">
       <c r="A73" s="58">
         <v>72</v>
       </c>
@@ -12192,7 +12216,7 @@
       <c r="V73" s="65"/>
       <c r="W73" s="65"/>
     </row>
-    <row r="74" spans="1:23" ht="80">
+    <row r="74" spans="1:23" ht="80" hidden="1">
       <c r="A74" s="63">
         <v>73</v>
       </c>
@@ -12259,7 +12283,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="144">
+    <row r="75" spans="1:23" ht="144" hidden="1">
       <c r="A75" s="58">
         <v>74</v>
       </c>
@@ -12328,7 +12352,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="80">
+    <row r="76" spans="1:23" ht="80" hidden="1">
       <c r="A76" s="63">
         <v>75</v>
       </c>
@@ -12393,7 +12417,7 @@
       <c r="V76" s="80"/>
       <c r="W76" s="80"/>
     </row>
-    <row r="77" spans="1:23" ht="48">
+    <row r="77" spans="1:23" ht="48" hidden="1">
       <c r="A77" s="63">
         <v>76</v>
       </c>
@@ -12456,7 +12480,7 @@
       <c r="V77" s="80"/>
       <c r="W77" s="80"/>
     </row>
-    <row r="78" spans="1:23" ht="64">
+    <row r="78" spans="1:23" ht="64" hidden="1">
       <c r="A78" s="63">
         <v>77</v>
       </c>
@@ -12521,7 +12545,7 @@
       </c>
       <c r="W78" s="80"/>
     </row>
-    <row r="79" spans="1:23" ht="48">
+    <row r="79" spans="1:23" ht="48" hidden="1">
       <c r="A79" s="58">
         <v>78</v>
       </c>
@@ -12588,7 +12612,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="32">
+    <row r="80" spans="1:23" ht="32" hidden="1">
       <c r="A80" s="96">
         <v>79</v>
       </c>
@@ -12653,7 +12677,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="32">
+    <row r="81" spans="1:23" ht="32" hidden="1">
       <c r="A81" s="63">
         <v>80</v>
       </c>
@@ -12716,7 +12740,7 @@
       <c r="V81" s="80"/>
       <c r="W81" s="80"/>
     </row>
-    <row r="82" spans="1:23" ht="32">
+    <row r="82" spans="1:23" ht="32" hidden="1">
       <c r="A82" s="58">
         <v>81</v>
       </c>
@@ -12779,7 +12803,7 @@
       <c r="V82" s="80"/>
       <c r="W82" s="80"/>
     </row>
-    <row r="83" spans="1:23" ht="144">
+    <row r="83" spans="1:23" ht="144" hidden="1">
       <c r="A83" s="63">
         <v>82</v>
       </c>
@@ -12848,7 +12872,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="80">
+    <row r="84" spans="1:23" ht="80" hidden="1">
       <c r="A84" s="63">
         <v>83</v>
       </c>
@@ -12913,7 +12937,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="32">
+    <row r="85" spans="1:23" ht="32" hidden="1">
       <c r="A85" s="63">
         <v>84</v>
       </c>
@@ -12982,7 +13006,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="32">
+    <row r="86" spans="1:23" ht="32" hidden="1">
       <c r="A86" s="58">
         <v>85</v>
       </c>
@@ -13051,7 +13075,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="32">
+    <row r="87" spans="1:23" ht="32" hidden="1">
       <c r="A87" s="63">
         <v>86</v>
       </c>
@@ -13120,7 +13144,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="80">
+    <row r="88" spans="1:23" ht="80" hidden="1">
       <c r="A88" s="63">
         <v>87</v>
       </c>
@@ -13189,7 +13213,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="64">
+    <row r="89" spans="1:23" ht="64" hidden="1">
       <c r="A89" s="63">
         <v>88</v>
       </c>
@@ -13232,7 +13256,7 @@
       </c>
       <c r="W89" s="69"/>
     </row>
-    <row r="90" spans="1:23" ht="48">
+    <row r="90" spans="1:23" ht="48" hidden="1">
       <c r="A90" s="58">
         <v>89</v>
       </c>
@@ -13277,7 +13301,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="48">
+    <row r="91" spans="1:23" ht="48" hidden="1">
       <c r="A91" s="63">
         <v>90</v>
       </c>
@@ -13322,7 +13346,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="64">
+    <row r="92" spans="1:23" ht="64" hidden="1">
       <c r="A92" s="63">
         <v>91</v>
       </c>
@@ -13391,7 +13415,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="34">
+    <row r="93" spans="1:23" ht="34" hidden="1">
       <c r="A93" s="58">
         <v>92</v>
       </c>
@@ -13458,7 +13482,7 @@
       </c>
       <c r="W93" s="69"/>
     </row>
-    <row r="94" spans="1:23" ht="32">
+    <row r="94" spans="1:23" ht="32" hidden="1">
       <c r="A94" s="58">
         <v>93</v>
       </c>
@@ -13521,7 +13545,7 @@
       </c>
       <c r="W94" s="69"/>
     </row>
-    <row r="95" spans="1:23" ht="32">
+    <row r="95" spans="1:23" ht="32" hidden="1">
       <c r="A95" s="58">
         <v>94</v>
       </c>
@@ -13588,7 +13612,7 @@
       </c>
       <c r="W95" s="69"/>
     </row>
-    <row r="96" spans="1:23" ht="32">
+    <row r="96" spans="1:23" ht="32" hidden="1">
       <c r="A96" s="58">
         <v>95</v>
       </c>
@@ -13651,7 +13675,7 @@
       </c>
       <c r="W96" s="69"/>
     </row>
-    <row r="97" spans="1:23" ht="32">
+    <row r="97" spans="1:23" ht="32" hidden="1">
       <c r="A97" s="58">
         <v>96</v>
       </c>
@@ -13718,7 +13742,7 @@
       </c>
       <c r="W97" s="69"/>
     </row>
-    <row r="98" spans="1:23" ht="32">
+    <row r="98" spans="1:23" ht="32" hidden="1">
       <c r="A98" s="58">
         <v>97</v>
       </c>
@@ -13781,7 +13805,7 @@
       </c>
       <c r="W98" s="69"/>
     </row>
-    <row r="99" spans="1:23" ht="96">
+    <row r="99" spans="1:23" ht="96" hidden="1">
       <c r="A99" s="63">
         <v>98</v>
       </c>
@@ -13848,7 +13872,7 @@
       </c>
       <c r="W99" s="80"/>
     </row>
-    <row r="100" spans="1:23" ht="80">
+    <row r="100" spans="1:23" ht="80" hidden="1">
       <c r="A100" s="63">
         <v>99</v>
       </c>
@@ -13911,7 +13935,7 @@
       <c r="V100" s="69"/>
       <c r="W100" s="69"/>
     </row>
-    <row r="101" spans="1:23" ht="48">
+    <row r="101" spans="1:23" ht="48" hidden="1">
       <c r="A101" s="63">
         <v>100</v>
       </c>
@@ -14014,7 +14038,7 @@
         <v>105</v>
       </c>
       <c r="K102" s="9" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="L102" s="6" t="s">
         <v>105</v>
@@ -14053,7 +14077,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="48">
+    <row r="103" spans="1:23" ht="64">
       <c r="A103" s="63">
         <v>102</v>
       </c>
@@ -14085,7 +14109,7 @@
         <v>105</v>
       </c>
       <c r="K103" s="109" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="L103" t="s">
         <v>105</v>
@@ -14124,7 +14148,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="80">
+    <row r="104" spans="1:23" ht="80" hidden="1">
       <c r="A104" s="58">
         <v>103</v>
       </c>
@@ -14193,7 +14217,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="32">
+    <row r="105" spans="1:23" ht="32" hidden="1">
       <c r="A105" s="63">
         <v>104</v>
       </c>
@@ -14225,7 +14249,7 @@
         <v>696</v>
       </c>
       <c r="K105" s="80" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="L105" s="98">
         <v>29290</v>
@@ -14293,8 +14317,8 @@
       <c r="J106" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="K106" s="80" t="s">
-        <v>854</v>
+      <c r="K106" s="112" t="s">
+        <v>855</v>
       </c>
       <c r="L106" s="80" t="s">
         <v>105</v>
@@ -14364,7 +14388,9 @@
       <c r="J107" s="80" t="s">
         <v>105</v>
       </c>
-      <c r="K107" s="80"/>
+      <c r="K107" s="112" t="s">
+        <v>856</v>
+      </c>
       <c r="L107" s="80" t="s">
         <v>105</v>
       </c>
@@ -14402,7 +14428,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="64">
+    <row r="108" spans="1:23" ht="64" hidden="1">
       <c r="A108" s="58">
         <v>107</v>
       </c>
@@ -14433,7 +14459,9 @@
       <c r="J108" s="69" t="s">
         <v>825</v>
       </c>
-      <c r="K108" s="69"/>
+      <c r="K108" s="69" t="s">
+        <v>857</v>
+      </c>
       <c r="L108" s="69">
         <v>50453.073400000001</v>
       </c>
@@ -14469,7 +14497,7 @@
       </c>
       <c r="W108" s="69"/>
     </row>
-    <row r="109" spans="1:23" ht="64">
+    <row r="109" spans="1:23" ht="64" hidden="1">
       <c r="A109" s="58">
         <v>107</v>
       </c>
@@ -14500,7 +14528,9 @@
       <c r="J109" s="69" t="s">
         <v>826</v>
       </c>
-      <c r="K109" s="69"/>
+      <c r="K109" s="69" t="s">
+        <v>857</v>
+      </c>
       <c r="L109" s="69" t="s">
         <v>824</v>
       </c>
@@ -14536,7 +14566,7 @@
       </c>
       <c r="W109" s="69"/>
     </row>
-    <row r="110" spans="1:23" ht="64">
+    <row r="110" spans="1:23" ht="64" hidden="1">
       <c r="A110" s="58">
         <v>107</v>
       </c>
@@ -14567,7 +14597,9 @@
       <c r="J110" s="69" t="s">
         <v>827</v>
       </c>
-      <c r="K110" s="69"/>
+      <c r="K110" s="69" t="s">
+        <v>857</v>
+      </c>
       <c r="L110" s="69" t="s">
         <v>180</v>
       </c>
@@ -14603,7 +14635,7 @@
       </c>
       <c r="W110" s="69"/>
     </row>
-    <row r="111" spans="1:23" ht="64">
+    <row r="111" spans="1:23" ht="64" hidden="1">
       <c r="A111" s="58">
         <v>107</v>
       </c>
@@ -14634,7 +14666,9 @@
       <c r="J111" s="69" t="s">
         <v>829</v>
       </c>
-      <c r="K111" s="69"/>
+      <c r="K111" s="69" t="s">
+        <v>857</v>
+      </c>
       <c r="L111" s="69" t="s">
         <v>830</v>
       </c>
@@ -14670,7 +14704,7 @@
       </c>
       <c r="W111" s="80"/>
     </row>
-    <row r="112" spans="1:23" ht="80">
+    <row r="112" spans="1:23" ht="80" hidden="1">
       <c r="A112" s="58">
         <v>108</v>
       </c>
@@ -14735,7 +14769,7 @@
       <c r="V112" s="69"/>
       <c r="W112" s="80"/>
     </row>
-    <row r="113" spans="1:23" ht="160">
+    <row r="113" spans="1:23" ht="160" hidden="1">
       <c r="A113" s="58">
         <v>109</v>
       </c>
@@ -14804,7 +14838,7 @@
       </c>
       <c r="W113" s="69"/>
     </row>
-    <row r="114" spans="1:23" ht="48">
+    <row r="114" spans="1:23" ht="48" hidden="1">
       <c r="A114" s="63">
         <v>110</v>
       </c>
@@ -14835,7 +14869,9 @@
       <c r="J114" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="K114" s="65"/>
+      <c r="K114" s="65" t="s">
+        <v>858</v>
+      </c>
       <c r="L114" s="80" t="s">
         <v>729</v>
       </c>
@@ -14871,7 +14907,7 @@
       </c>
       <c r="W114" s="80"/>
     </row>
-    <row r="115" spans="1:23" ht="64">
+    <row r="115" spans="1:23" ht="64" hidden="1">
       <c r="A115" s="63">
         <v>111</v>
       </c>
@@ -14942,7 +14978,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="64">
+    <row r="116" spans="1:23" ht="64" hidden="1">
       <c r="A116" s="63">
         <v>112</v>
       </c>
@@ -15013,7 +15049,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="112">
+    <row r="117" spans="1:23" ht="112" hidden="1">
       <c r="A117" s="63">
         <v>113</v>
       </c>
@@ -15084,7 +15120,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="176">
+    <row r="118" spans="1:23" ht="176" hidden="1">
       <c r="A118" s="63">
         <v>114</v>
       </c>
@@ -15153,7 +15189,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="32">
+    <row r="119" spans="1:23" ht="32" hidden="1">
       <c r="A119" s="63">
         <v>118</v>
       </c>
@@ -15222,7 +15258,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="80">
+    <row r="120" spans="1:23" ht="80" hidden="1">
       <c r="A120" s="58">
         <v>119</v>
       </c>
@@ -15289,7 +15325,7 @@
       </c>
       <c r="W120" s="69"/>
     </row>
-    <row r="121" spans="1:23" ht="48">
+    <row r="121" spans="1:23" ht="48" hidden="1">
       <c r="A121" s="63">
         <v>120</v>
       </c>
@@ -15320,7 +15356,9 @@
       <c r="J121" s="80" t="s">
         <v>810</v>
       </c>
-      <c r="K121" s="80"/>
+      <c r="K121" s="80" t="s">
+        <v>845</v>
+      </c>
       <c r="L121" s="80" t="s">
         <v>180</v>
       </c>
@@ -16585,9 +16623,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16756,19 +16797,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6ECE83-F240-478D-BE60-3B98A1630AA1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91500E67-CFBD-4E57-93CA-25297AD67667}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16793,9 +16830,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91500E67-CFBD-4E57-93CA-25297AD67667}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6ECE83-F240-478D-BE60-3B98A1630AA1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>